<commit_message>
global and us updated 29 march
</commit_message>
<xml_diff>
--- a/mac_us_states_deaths.xlsx
+++ b/mac_us_states_deaths.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="262" documentId="8_{01E479FA-0407-4188-80FA-D8939889E2E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0C266511-B0A6-426E-8DF5-9A37D93ECBE5}"/>
+  <xr:revisionPtr revIDLastSave="285" documentId="8_{01E479FA-0407-4188-80FA-D8939889E2E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{89BB4B4F-0067-4756-A7D3-417E8178015B}"/>
   <bookViews>
-    <workbookView xWindow="6795" yWindow="-19080" windowWidth="22020" windowHeight="12945" xr2:uid="{479F01FD-FBEA-480D-8311-3224064F669A}"/>
+    <workbookView xWindow="8040" yWindow="-18150" windowWidth="13155" windowHeight="13245" xr2:uid="{479F01FD-FBEA-480D-8311-3224064F669A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>New York</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>Wyoming</t>
+  </si>
+  <si>
+    <t>3/28/20</t>
   </si>
 </sst>
 </file>
@@ -292,7 +295,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -301,9 +304,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -631,14 +631,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C58A35-5762-462F-A8C8-AA6852158F40}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="7.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="15" width="7.453125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
@@ -675,20 +675,20 @@
       <c r="K1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>54</v>
+      <c r="L1" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="P1" s="4" t="s">
         <v>58</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
@@ -725,20 +725,20 @@
       <c r="K2" s="3">
         <v>0</v>
       </c>
-      <c r="L2" s="5">
-        <v>0</v>
-      </c>
-      <c r="M2" s="5">
-        <v>0</v>
-      </c>
-      <c r="N2" s="5">
-        <v>0</v>
-      </c>
-      <c r="O2" s="5">
-        <v>1</v>
-      </c>
-      <c r="P2" s="2">
-        <v>1</v>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
@@ -782,12 +782,12 @@
         <v>0</v>
       </c>
       <c r="N3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="3">
-        <v>1</v>
-      </c>
-      <c r="P3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3">
         <v>1</v>
       </c>
     </row>
@@ -825,20 +825,20 @@
       <c r="K4" s="3">
         <v>2</v>
       </c>
-      <c r="L4" s="5">
-        <v>2</v>
-      </c>
-      <c r="M4" s="5">
+      <c r="L4" s="4">
         <v>5</v>
       </c>
-      <c r="N4" s="5">
+      <c r="M4" s="4">
         <v>6</v>
       </c>
-      <c r="O4" s="5">
+      <c r="N4" s="4">
         <v>8</v>
       </c>
-      <c r="P4" s="2">
+      <c r="O4" s="2">
         <v>8</v>
+      </c>
+      <c r="P4">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
@@ -875,20 +875,20 @@
       <c r="K5" s="3">
         <v>0</v>
       </c>
-      <c r="L5" s="5">
-        <v>0</v>
-      </c>
-      <c r="M5" s="5">
-        <v>0</v>
-      </c>
-      <c r="N5" s="5">
-        <v>2</v>
-      </c>
-      <c r="O5" s="5">
-        <v>3</v>
-      </c>
-      <c r="P5" s="2">
-        <v>3</v>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>2</v>
+      </c>
+      <c r="N5" s="4">
+        <v>3</v>
+      </c>
+      <c r="O5" s="2">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
@@ -925,20 +925,20 @@
       <c r="K6" s="3">
         <v>30</v>
       </c>
-      <c r="L6" s="5">
-        <v>27</v>
-      </c>
-      <c r="M6" s="5">
+      <c r="L6" s="4">
         <v>40</v>
       </c>
-      <c r="N6" s="5">
+      <c r="M6" s="4">
         <v>53</v>
       </c>
-      <c r="O6" s="5">
+      <c r="N6" s="4">
         <v>65</v>
       </c>
-      <c r="P6" s="2">
+      <c r="O6" s="2">
         <v>81</v>
+      </c>
+      <c r="P6">
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
@@ -975,20 +975,20 @@
       <c r="K7" s="3">
         <v>6</v>
       </c>
-      <c r="L7" s="5">
-        <v>6</v>
-      </c>
-      <c r="M7" s="5">
+      <c r="L7" s="4">
         <v>7</v>
       </c>
-      <c r="N7" s="5">
+      <c r="M7" s="4">
         <v>11</v>
       </c>
-      <c r="O7" s="5">
+      <c r="N7" s="4">
         <v>24</v>
       </c>
-      <c r="P7" s="2">
+      <c r="O7" s="2">
         <v>24</v>
+      </c>
+      <c r="P7">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
@@ -1025,20 +1025,20 @@
       <c r="K8" s="3">
         <v>5</v>
       </c>
-      <c r="L8" s="5">
-        <v>10</v>
-      </c>
-      <c r="M8" s="5">
+      <c r="L8" s="4">
         <v>12</v>
       </c>
-      <c r="N8" s="5">
+      <c r="M8" s="4">
         <v>19</v>
       </c>
-      <c r="O8" s="5">
+      <c r="N8" s="4">
         <v>21</v>
       </c>
-      <c r="P8" s="2">
+      <c r="O8" s="2">
         <v>21</v>
+      </c>
+      <c r="P8">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
@@ -1075,20 +1075,20 @@
       <c r="K9" s="3">
         <v>0</v>
       </c>
-      <c r="L9" s="5">
-        <v>0</v>
-      </c>
-      <c r="M9" s="5">
-        <v>0</v>
-      </c>
-      <c r="N9" s="5">
-        <v>0</v>
-      </c>
-      <c r="O9" s="5">
-        <v>2</v>
-      </c>
-      <c r="P9" s="2">
-        <v>2</v>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>2</v>
+      </c>
+      <c r="O9" s="2">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
@@ -1125,20 +1125,20 @@
       <c r="K10" s="3">
         <v>2</v>
       </c>
-      <c r="L10" s="5">
-        <v>2</v>
-      </c>
-      <c r="M10" s="5">
-        <v>2</v>
-      </c>
-      <c r="N10" s="5">
-        <v>2</v>
-      </c>
-      <c r="O10" s="5">
-        <v>3</v>
-      </c>
-      <c r="P10" s="2">
-        <v>3</v>
+      <c r="L10" s="4">
+        <v>2</v>
+      </c>
+      <c r="M10" s="4">
+        <v>2</v>
+      </c>
+      <c r="N10" s="4">
+        <v>3</v>
+      </c>
+      <c r="O10" s="2">
+        <v>3</v>
+      </c>
+      <c r="P10">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
@@ -1175,20 +1175,20 @@
       <c r="K11" s="3">
         <v>13</v>
       </c>
-      <c r="L11" s="5">
-        <v>14</v>
-      </c>
-      <c r="M11" s="5">
+      <c r="L11" s="4">
         <v>18</v>
       </c>
-      <c r="N11" s="5">
+      <c r="M11" s="4">
         <v>22</v>
       </c>
-      <c r="O11" s="5">
+      <c r="N11" s="4">
         <v>29</v>
       </c>
-      <c r="P11" s="2">
+      <c r="O11" s="2">
         <v>29</v>
+      </c>
+      <c r="P11">
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
@@ -1225,20 +1225,20 @@
       <c r="K12" s="3">
         <v>23</v>
       </c>
-      <c r="L12" s="5">
-        <v>25</v>
-      </c>
-      <c r="M12" s="5">
+      <c r="L12" s="4">
         <v>32</v>
       </c>
-      <c r="N12" s="5">
+      <c r="M12" s="4">
         <v>40</v>
       </c>
-      <c r="O12" s="5">
+      <c r="N12" s="4">
         <v>56</v>
       </c>
-      <c r="P12" s="2">
+      <c r="O12" s="2">
         <v>56</v>
+      </c>
+      <c r="P12">
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
@@ -1275,19 +1275,19 @@
       <c r="K13" s="3">
         <v>0</v>
       </c>
-      <c r="L13" s="5">
-        <v>1</v>
-      </c>
-      <c r="M13" s="5">
-        <v>1</v>
-      </c>
-      <c r="N13" s="5">
-        <v>1</v>
-      </c>
-      <c r="O13" s="5">
-        <v>1</v>
-      </c>
-      <c r="P13" s="2">
+      <c r="L13" s="4">
+        <v>1</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+      <c r="N13" s="4">
+        <v>1</v>
+      </c>
+      <c r="O13" s="2">
+        <v>1</v>
+      </c>
+      <c r="P13">
         <v>1</v>
       </c>
     </row>
@@ -1332,13 +1332,13 @@
         <v>0</v>
       </c>
       <c r="N14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
@@ -1375,20 +1375,20 @@
       <c r="K15" s="3">
         <v>0</v>
       </c>
-      <c r="L15" s="5">
-        <v>0</v>
-      </c>
-      <c r="M15" s="5">
-        <v>0</v>
-      </c>
-      <c r="N15" s="5">
-        <v>0</v>
-      </c>
-      <c r="O15" s="5">
-        <v>3</v>
-      </c>
-      <c r="P15" s="2">
-        <v>3</v>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>3</v>
+      </c>
+      <c r="O15" s="2">
+        <v>3</v>
+      </c>
+      <c r="P15">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
@@ -1425,20 +1425,20 @@
       <c r="K16" s="3">
         <v>9</v>
       </c>
-      <c r="L16" s="5">
-        <v>12</v>
-      </c>
-      <c r="M16" s="5">
+      <c r="L16" s="4">
         <v>16</v>
       </c>
-      <c r="N16" s="5">
+      <c r="M16" s="4">
         <v>19</v>
       </c>
-      <c r="O16" s="5">
+      <c r="N16" s="4">
         <v>26</v>
       </c>
-      <c r="P16" s="2">
+      <c r="O16" s="2">
         <v>26</v>
+      </c>
+      <c r="P16">
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
@@ -1475,20 +1475,20 @@
       <c r="K17" s="3">
         <v>6</v>
       </c>
-      <c r="L17" s="5">
-        <v>7</v>
-      </c>
-      <c r="M17" s="5">
+      <c r="L17" s="4">
         <v>12</v>
       </c>
-      <c r="N17" s="5">
+      <c r="M17" s="4">
         <v>14</v>
       </c>
-      <c r="O17" s="5">
+      <c r="N17" s="4">
         <v>17</v>
       </c>
-      <c r="P17" s="2">
+      <c r="O17" s="2">
         <v>18</v>
+      </c>
+      <c r="P17">
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
@@ -1525,20 +1525,20 @@
       <c r="K18" s="3">
         <v>0</v>
       </c>
-      <c r="L18" s="5">
-        <v>0</v>
-      </c>
-      <c r="M18" s="5">
-        <v>0</v>
-      </c>
-      <c r="N18" s="5">
-        <v>1</v>
-      </c>
-      <c r="O18" s="5">
-        <v>1</v>
-      </c>
-      <c r="P18" s="2">
-        <v>1</v>
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4">
+        <v>1</v>
+      </c>
+      <c r="N18" s="4">
+        <v>1</v>
+      </c>
+      <c r="O18" s="2">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
@@ -1575,20 +1575,20 @@
       <c r="K19" s="3">
         <v>2</v>
       </c>
-      <c r="L19" s="5">
-        <v>2</v>
-      </c>
-      <c r="M19" s="5">
-        <v>2</v>
-      </c>
-      <c r="N19" s="5">
-        <v>3</v>
-      </c>
-      <c r="O19" s="5">
-        <v>3</v>
-      </c>
-      <c r="P19" s="2">
-        <v>3</v>
+      <c r="L19" s="4">
+        <v>2</v>
+      </c>
+      <c r="M19" s="4">
+        <v>3</v>
+      </c>
+      <c r="N19" s="4">
+        <v>3</v>
+      </c>
+      <c r="O19" s="2">
+        <v>3</v>
+      </c>
+      <c r="P19">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
@@ -1625,20 +1625,20 @@
       <c r="K20" s="3">
         <v>3</v>
       </c>
-      <c r="L20" s="5">
-        <v>3</v>
-      </c>
-      <c r="M20" s="5">
+      <c r="L20" s="4">
         <v>4</v>
       </c>
-      <c r="N20" s="5">
+      <c r="M20" s="4">
         <v>4</v>
       </c>
-      <c r="O20" s="5">
+      <c r="N20" s="4">
         <v>5</v>
       </c>
-      <c r="P20" s="2">
+      <c r="O20" s="2">
         <v>5</v>
+      </c>
+      <c r="P20">
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
@@ -1675,20 +1675,20 @@
       <c r="K21" s="3">
         <v>20</v>
       </c>
-      <c r="L21" s="5">
-        <v>34</v>
-      </c>
-      <c r="M21" s="5">
+      <c r="L21" s="4">
         <v>46</v>
       </c>
-      <c r="N21" s="5">
+      <c r="M21" s="4">
         <v>65</v>
       </c>
-      <c r="O21" s="5">
+      <c r="N21" s="4">
         <v>83</v>
       </c>
-      <c r="P21" s="2">
+      <c r="O21" s="2">
         <v>83</v>
+      </c>
+      <c r="P21">
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
@@ -1737,8 +1737,8 @@
       <c r="O22" s="3">
         <v>0</v>
       </c>
-      <c r="P22" s="3">
-        <v>0</v>
+      <c r="P22">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
@@ -1775,20 +1775,20 @@
       <c r="K23" s="3">
         <v>3</v>
       </c>
-      <c r="L23" s="5">
-        <v>3</v>
-      </c>
-      <c r="M23" s="5">
-        <v>3</v>
-      </c>
-      <c r="N23" s="5">
+      <c r="L23" s="4">
+        <v>3</v>
+      </c>
+      <c r="M23" s="4">
         <v>4</v>
       </c>
-      <c r="O23" s="5">
+      <c r="N23" s="4">
         <v>4</v>
       </c>
-      <c r="P23" s="2">
+      <c r="O23" s="2">
         <v>4</v>
+      </c>
+      <c r="P23">
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
@@ -1825,20 +1825,20 @@
       <c r="K24" s="3">
         <v>5</v>
       </c>
-      <c r="L24" s="5">
-        <v>9</v>
-      </c>
-      <c r="M24" s="5">
+      <c r="L24" s="4">
         <v>11</v>
       </c>
-      <c r="N24" s="5">
+      <c r="M24" s="4">
         <v>15</v>
       </c>
-      <c r="O24" s="5">
+      <c r="N24" s="4">
         <v>25</v>
       </c>
-      <c r="P24" s="2">
+      <c r="O24" s="2">
         <v>25</v>
+      </c>
+      <c r="P24">
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
@@ -1875,20 +1875,20 @@
       <c r="K25" s="3">
         <v>9</v>
       </c>
-      <c r="L25" s="5">
-        <v>15</v>
-      </c>
-      <c r="M25" s="5">
+      <c r="L25" s="4">
         <v>24</v>
       </c>
-      <c r="N25" s="5">
+      <c r="M25" s="4">
         <v>43</v>
       </c>
-      <c r="O25" s="5">
+      <c r="N25" s="4">
         <v>60</v>
       </c>
-      <c r="P25" s="2">
+      <c r="O25" s="2">
         <v>63</v>
+      </c>
+      <c r="P25">
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
@@ -1925,20 +1925,20 @@
       <c r="K26" s="3">
         <v>1</v>
       </c>
-      <c r="L26" s="5">
-        <v>1</v>
-      </c>
-      <c r="M26" s="5">
-        <v>1</v>
-      </c>
-      <c r="N26" s="5">
-        <v>1</v>
-      </c>
-      <c r="O26" s="5">
-        <v>2</v>
-      </c>
-      <c r="P26" s="2">
-        <v>2</v>
+      <c r="L26" s="4">
+        <v>1</v>
+      </c>
+      <c r="M26" s="4">
+        <v>1</v>
+      </c>
+      <c r="N26" s="4">
+        <v>2</v>
+      </c>
+      <c r="O26" s="2">
+        <v>2</v>
+      </c>
+      <c r="P26">
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
@@ -1975,20 +1975,20 @@
       <c r="K27" s="3">
         <v>1</v>
       </c>
-      <c r="L27" s="5">
-        <v>1</v>
-      </c>
-      <c r="M27" s="5">
-        <v>1</v>
-      </c>
-      <c r="N27" s="5">
-        <v>2</v>
-      </c>
-      <c r="O27" s="5">
+      <c r="L27" s="4">
+        <v>1</v>
+      </c>
+      <c r="M27" s="4">
+        <v>2</v>
+      </c>
+      <c r="N27" s="4">
         <v>6</v>
       </c>
-      <c r="P27" s="2">
+      <c r="O27" s="2">
         <v>6</v>
+      </c>
+      <c r="P27">
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
@@ -2025,20 +2025,20 @@
       <c r="K28" s="3">
         <v>3</v>
       </c>
-      <c r="L28" s="5">
-        <v>3</v>
-      </c>
-      <c r="M28" s="5">
-        <v>3</v>
-      </c>
-      <c r="N28" s="5">
+      <c r="L28" s="4">
+        <v>3</v>
+      </c>
+      <c r="M28" s="4">
         <v>8</v>
       </c>
-      <c r="O28" s="5">
+      <c r="N28" s="4">
         <v>8</v>
       </c>
-      <c r="P28" s="2">
+      <c r="O28" s="2">
         <v>8</v>
+      </c>
+      <c r="P28">
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
@@ -2087,8 +2087,8 @@
       <c r="O29" s="3">
         <v>0</v>
       </c>
-      <c r="P29" s="3">
-        <v>0</v>
+      <c r="P29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
@@ -2137,8 +2137,8 @@
       <c r="O30" s="3">
         <v>0</v>
       </c>
-      <c r="P30" s="3">
-        <v>0</v>
+      <c r="P30">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
@@ -2175,20 +2175,20 @@
       <c r="K31" s="3">
         <v>2</v>
       </c>
-      <c r="L31" s="5">
+      <c r="L31" s="4">
         <v>4</v>
       </c>
-      <c r="M31" s="5">
-        <v>4</v>
-      </c>
-      <c r="N31" s="5">
+      <c r="M31" s="4">
         <v>6</v>
       </c>
-      <c r="O31" s="5">
+      <c r="N31" s="4">
         <v>10</v>
       </c>
-      <c r="P31" s="2">
+      <c r="O31" s="2">
         <v>10</v>
+      </c>
+      <c r="P31">
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
@@ -2225,20 +2225,20 @@
       <c r="K32" s="3">
         <v>0</v>
       </c>
-      <c r="L32" s="5">
-        <v>0</v>
-      </c>
-      <c r="M32" s="5">
-        <v>1</v>
-      </c>
-      <c r="N32" s="5">
-        <v>1</v>
-      </c>
-      <c r="O32" s="5">
-        <v>1</v>
-      </c>
-      <c r="P32" s="2">
-        <v>1</v>
+      <c r="L32" s="4">
+        <v>1</v>
+      </c>
+      <c r="M32" s="4">
+        <v>1</v>
+      </c>
+      <c r="N32" s="4">
+        <v>1</v>
+      </c>
+      <c r="O32" s="2">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.35">
@@ -2275,20 +2275,20 @@
       <c r="K33" s="3">
         <v>20</v>
       </c>
-      <c r="L33" s="5">
-        <v>27</v>
-      </c>
-      <c r="M33" s="5">
+      <c r="L33" s="4">
         <v>44</v>
       </c>
-      <c r="N33" s="5">
+      <c r="M33" s="4">
         <v>62</v>
       </c>
-      <c r="O33" s="5">
+      <c r="N33" s="4">
         <v>81</v>
       </c>
-      <c r="P33" s="2">
+      <c r="O33" s="2">
         <v>81</v>
+      </c>
+      <c r="P33">
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.35">
@@ -2325,20 +2325,20 @@
       <c r="K34" s="3">
         <v>0</v>
       </c>
-      <c r="L34" s="5">
-        <v>0</v>
-      </c>
-      <c r="M34" s="5">
-        <v>0</v>
-      </c>
-      <c r="N34" s="5">
-        <v>1</v>
-      </c>
-      <c r="O34" s="5">
-        <v>1</v>
-      </c>
-      <c r="P34" s="2">
-        <v>1</v>
+      <c r="L34" s="4">
+        <v>0</v>
+      </c>
+      <c r="M34" s="4">
+        <v>1</v>
+      </c>
+      <c r="N34" s="4">
+        <v>1</v>
+      </c>
+      <c r="O34" s="2">
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
@@ -2375,20 +2375,20 @@
       <c r="K35" s="3">
         <v>117</v>
       </c>
-      <c r="L35" s="5">
-        <v>114</v>
-      </c>
-      <c r="M35" s="5">
+      <c r="L35" s="4">
         <v>210</v>
       </c>
-      <c r="N35" s="5">
+      <c r="M35" s="4">
         <v>285</v>
       </c>
-      <c r="O35" s="5">
+      <c r="N35" s="4">
         <v>385</v>
       </c>
-      <c r="P35" s="2">
+      <c r="O35" s="2">
         <v>432</v>
+      </c>
+      <c r="P35">
+        <v>782</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
@@ -2425,20 +2425,20 @@
       <c r="K36" s="3">
         <v>0</v>
       </c>
-      <c r="L36" s="5">
-        <v>0</v>
-      </c>
-      <c r="M36" s="5">
-        <v>0</v>
-      </c>
-      <c r="N36" s="5">
-        <v>1</v>
-      </c>
-      <c r="O36" s="5">
-        <v>2</v>
-      </c>
-      <c r="P36" s="2">
-        <v>2</v>
+      <c r="L36" s="4">
+        <v>0</v>
+      </c>
+      <c r="M36" s="4">
+        <v>1</v>
+      </c>
+      <c r="N36" s="4">
+        <v>2</v>
+      </c>
+      <c r="O36" s="2">
+        <v>2</v>
+      </c>
+      <c r="P36">
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
@@ -2487,8 +2487,8 @@
       <c r="O37" s="3">
         <v>0</v>
       </c>
-      <c r="P37" s="3">
-        <v>0</v>
+      <c r="P37">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.35">
@@ -2525,20 +2525,20 @@
       <c r="K38" s="3">
         <v>3</v>
       </c>
-      <c r="L38" s="5">
-        <v>6</v>
-      </c>
-      <c r="M38" s="5">
+      <c r="L38" s="4">
         <v>8</v>
       </c>
-      <c r="N38" s="5">
+      <c r="M38" s="4">
         <v>10</v>
       </c>
-      <c r="O38" s="5">
+      <c r="N38" s="4">
         <v>15</v>
       </c>
-      <c r="P38" s="2">
+      <c r="O38" s="2">
         <v>15</v>
+      </c>
+      <c r="P38">
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.35">
@@ -2575,20 +2575,20 @@
       <c r="K39" s="3">
         <v>2</v>
       </c>
-      <c r="L39" s="5">
-        <v>2</v>
-      </c>
-      <c r="M39" s="5">
-        <v>3</v>
-      </c>
-      <c r="N39" s="5">
+      <c r="L39" s="4">
+        <v>3</v>
+      </c>
+      <c r="M39" s="4">
         <v>5</v>
       </c>
-      <c r="O39" s="5">
+      <c r="N39" s="4">
         <v>7</v>
       </c>
-      <c r="P39" s="2">
+      <c r="O39" s="2">
         <v>7</v>
+      </c>
+      <c r="P39">
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.35">
@@ -2625,20 +2625,20 @@
       <c r="K40" s="3">
         <v>4</v>
       </c>
-      <c r="L40" s="5">
-        <v>5</v>
-      </c>
-      <c r="M40" s="5">
+      <c r="L40" s="4">
         <v>8</v>
       </c>
-      <c r="N40" s="5">
+      <c r="M40" s="4">
         <v>8</v>
       </c>
-      <c r="O40" s="5">
+      <c r="N40" s="4">
         <v>11</v>
       </c>
-      <c r="P40" s="2">
+      <c r="O40" s="2">
         <v>11</v>
+      </c>
+      <c r="P40">
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.35">
@@ -2675,20 +2675,20 @@
       <c r="K41" s="3">
         <v>3</v>
       </c>
-      <c r="L41" s="5">
-        <v>6</v>
-      </c>
-      <c r="M41" s="5">
+      <c r="L41" s="4">
         <v>7</v>
       </c>
-      <c r="N41" s="5">
+      <c r="M41" s="4">
         <v>11</v>
       </c>
-      <c r="O41" s="5">
+      <c r="N41" s="4">
         <v>16</v>
       </c>
-      <c r="P41" s="2">
+      <c r="O41" s="2">
         <v>16</v>
+      </c>
+      <c r="P41">
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.35">
@@ -2725,20 +2725,20 @@
       <c r="K42" s="3">
         <v>0</v>
       </c>
-      <c r="L42" s="5">
-        <v>2</v>
-      </c>
-      <c r="M42" s="5">
-        <v>2</v>
-      </c>
-      <c r="N42" s="5">
-        <v>2</v>
-      </c>
-      <c r="O42" s="5">
-        <v>2</v>
-      </c>
-      <c r="P42" s="2">
-        <v>2</v>
+      <c r="L42" s="4">
+        <v>2</v>
+      </c>
+      <c r="M42" s="4">
+        <v>2</v>
+      </c>
+      <c r="N42" s="4">
+        <v>2</v>
+      </c>
+      <c r="O42" s="2">
+        <v>2</v>
+      </c>
+      <c r="P42">
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.35">
@@ -2787,8 +2787,8 @@
       <c r="O43" s="3">
         <v>0</v>
       </c>
-      <c r="P43" s="3">
-        <v>0</v>
+      <c r="P43">
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.35">
@@ -2825,20 +2825,20 @@
       <c r="K44" s="3">
         <v>3</v>
       </c>
-      <c r="L44" s="5">
+      <c r="L44" s="4">
         <v>5</v>
       </c>
-      <c r="M44" s="5">
-        <v>5</v>
-      </c>
-      <c r="N44" s="5">
+      <c r="M44" s="4">
         <v>7</v>
       </c>
-      <c r="O44" s="5">
+      <c r="N44" s="4">
         <v>9</v>
       </c>
-      <c r="P44" s="2">
+      <c r="O44" s="2">
         <v>9</v>
+      </c>
+      <c r="P44">
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.35">
@@ -2884,10 +2884,10 @@
       <c r="N45" s="3">
         <v>1</v>
       </c>
-      <c r="O45" s="3">
-        <v>1</v>
-      </c>
-      <c r="P45" s="2">
+      <c r="O45" s="2">
+        <v>1</v>
+      </c>
+      <c r="P45">
         <v>1</v>
       </c>
     </row>
@@ -2925,20 +2925,20 @@
       <c r="K46" s="3">
         <v>2</v>
       </c>
-      <c r="L46" s="5">
-        <v>2</v>
-      </c>
-      <c r="M46" s="5">
-        <v>2</v>
-      </c>
-      <c r="N46" s="5">
-        <v>3</v>
-      </c>
-      <c r="O46" s="5">
-        <v>3</v>
-      </c>
-      <c r="P46" s="2">
-        <v>3</v>
+      <c r="L46" s="4">
+        <v>2</v>
+      </c>
+      <c r="M46" s="4">
+        <v>3</v>
+      </c>
+      <c r="N46" s="4">
+        <v>3</v>
+      </c>
+      <c r="O46" s="2">
+        <v>3</v>
+      </c>
+      <c r="P46">
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.35">
@@ -2975,20 +2975,20 @@
       <c r="K47" s="3">
         <v>6</v>
       </c>
-      <c r="L47" s="5">
-        <v>8</v>
-      </c>
-      <c r="M47" s="5">
+      <c r="L47" s="4">
         <v>9</v>
       </c>
-      <c r="N47" s="5">
+      <c r="M47" s="4">
         <v>12</v>
       </c>
-      <c r="O47" s="5">
+      <c r="N47" s="4">
         <v>18</v>
       </c>
-      <c r="P47" s="2">
+      <c r="O47" s="2">
         <v>21</v>
+      </c>
+      <c r="P47">
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.35">
@@ -3034,11 +3034,11 @@
       <c r="N48" s="3">
         <v>1</v>
       </c>
-      <c r="O48" s="3">
-        <v>1</v>
-      </c>
-      <c r="P48" s="2">
-        <v>1</v>
+      <c r="O48" s="2">
+        <v>1</v>
+      </c>
+      <c r="P48">
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.35">
@@ -3075,20 +3075,20 @@
       <c r="K49" s="3">
         <v>2</v>
       </c>
-      <c r="L49" s="5">
-        <v>5</v>
-      </c>
-      <c r="M49" s="5">
+      <c r="L49" s="4">
         <v>7</v>
       </c>
-      <c r="N49" s="5">
+      <c r="M49" s="4">
         <v>8</v>
       </c>
-      <c r="O49" s="5">
+      <c r="N49" s="4">
         <v>9</v>
       </c>
-      <c r="P49" s="2">
+      <c r="O49" s="2">
         <v>9</v>
+      </c>
+      <c r="P49">
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.35">
@@ -3125,20 +3125,20 @@
       <c r="K50" s="3">
         <v>6</v>
       </c>
-      <c r="L50" s="5">
-        <v>6</v>
-      </c>
-      <c r="M50" s="5">
+      <c r="L50" s="4">
         <v>7</v>
       </c>
-      <c r="N50" s="5">
+      <c r="M50" s="4">
         <v>9</v>
       </c>
-      <c r="O50" s="5">
+      <c r="N50" s="4">
         <v>13</v>
       </c>
-      <c r="P50" s="2">
+      <c r="O50" s="2">
         <v>13</v>
+      </c>
+      <c r="P50">
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.35">
@@ -3175,20 +3175,20 @@
       <c r="K51" s="3">
         <v>95</v>
       </c>
-      <c r="L51" s="5">
-        <v>95</v>
-      </c>
-      <c r="M51" s="5">
+      <c r="L51" s="4">
         <v>110</v>
       </c>
-      <c r="N51" s="5">
+      <c r="M51" s="4">
         <v>123</v>
       </c>
-      <c r="O51" s="5">
+      <c r="N51" s="4">
         <v>147</v>
       </c>
-      <c r="P51" s="2">
+      <c r="O51" s="2">
         <v>151</v>
+      </c>
+      <c r="P51">
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">
@@ -3275,20 +3275,20 @@
       <c r="K53" s="3">
         <v>4</v>
       </c>
-      <c r="L53" s="5">
+      <c r="L53" s="4">
         <v>5</v>
       </c>
-      <c r="M53" s="5">
-        <v>5</v>
-      </c>
-      <c r="N53" s="5">
+      <c r="M53" s="4">
         <v>7</v>
       </c>
-      <c r="O53" s="5">
+      <c r="N53" s="4">
         <v>8</v>
       </c>
-      <c r="P53" s="2">
+      <c r="O53" s="2">
         <v>10</v>
+      </c>
+      <c r="P53">
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.35">
@@ -3342,8 +3342,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P54" xr:uid="{6DBA1537-44B7-457D-A372-52F033B35063}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P54">
+  <autoFilter ref="A1:O54" xr:uid="{6DBA1537-44B7-457D-A372-52F033B35063}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O54">
       <sortCondition ref="A1:A54"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
30 March updates done
</commit_message>
<xml_diff>
--- a/mac_us_states_deaths.xlsx
+++ b/mac_us_states_deaths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="285" documentId="8_{01E479FA-0407-4188-80FA-D8939889E2E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{89BB4B4F-0067-4756-A7D3-417E8178015B}"/>
+  <xr:revisionPtr revIDLastSave="289" documentId="8_{01E479FA-0407-4188-80FA-D8939889E2E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0C1433FD-9DEA-45E7-9A64-893035226C85}"/>
   <bookViews>
-    <workbookView xWindow="8040" yWindow="-18150" windowWidth="13155" windowHeight="13245" xr2:uid="{479F01FD-FBEA-480D-8311-3224064F669A}"/>
+    <workbookView xWindow="9570" yWindow="-16620" windowWidth="13155" windowHeight="13245" xr2:uid="{479F01FD-FBEA-480D-8311-3224064F669A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>New York</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>3/28/20</t>
+  </si>
+  <si>
+    <t>3/29/20</t>
   </si>
 </sst>
 </file>
@@ -295,7 +298,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -307,6 +310,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -629,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C58A35-5762-462F-A8C8-AA6852158F40}">
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -641,7 +650,7 @@
     <col min="2" max="15" width="7.453125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -690,8 +699,11 @@
       <c r="P1" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q1" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -740,8 +752,11 @@
       <c r="P2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q2" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>62</v>
       </c>
@@ -790,8 +805,11 @@
       <c r="P3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -840,8 +858,11 @@
       <c r="P4">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q4" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -890,8 +911,11 @@
       <c r="P5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q5" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -940,8 +964,11 @@
       <c r="P6">
         <v>121</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q6" s="5">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -990,8 +1017,11 @@
       <c r="P7">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q7" s="5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1040,8 +1070,11 @@
       <c r="P8">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q8" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
@@ -1090,8 +1123,11 @@
       <c r="P9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q9" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1140,8 +1176,11 @@
       <c r="P10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q10" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1190,8 +1229,11 @@
       <c r="P11">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q11" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1240,8 +1282,11 @@
       <c r="P12">
         <v>79</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q12" s="5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -1290,8 +1335,11 @@
       <c r="P13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>61</v>
       </c>
@@ -1340,8 +1388,11 @@
       <c r="P14" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1390,8 +1441,11 @@
       <c r="P15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q15" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1440,8 +1494,11 @@
       <c r="P16">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q16" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1490,8 +1547,11 @@
       <c r="P17">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q17" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
@@ -1540,8 +1600,11 @@
       <c r="P18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q18" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1590,8 +1653,11 @@
       <c r="P19">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q19" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1640,8 +1706,11 @@
       <c r="P20">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q20" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -1690,8 +1759,11 @@
       <c r="P21">
         <v>137</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q21" s="5">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -1740,8 +1812,11 @@
       <c r="P22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q22" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1790,8 +1865,11 @@
       <c r="P23">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q23" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -1840,8 +1918,11 @@
       <c r="P24">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q24" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -1890,8 +1971,11 @@
       <c r="P25">
         <v>111</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q25" s="5">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -1940,8 +2024,11 @@
       <c r="P26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q26" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1990,8 +2077,11 @@
       <c r="P27">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q27" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -2040,8 +2130,11 @@
       <c r="P28">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q28" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>64</v>
       </c>
@@ -2090,8 +2183,11 @@
       <c r="P29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q29" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>59</v>
       </c>
@@ -2140,8 +2236,11 @@
       <c r="P30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q30" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
@@ -2190,8 +2289,11 @@
       <c r="P31">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q31" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
@@ -2240,8 +2342,11 @@
       <c r="P32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q32" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
@@ -2290,8 +2395,11 @@
       <c r="P33">
         <v>140</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q33" s="5">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -2340,8 +2448,11 @@
       <c r="P34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q34" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -2390,8 +2501,11 @@
       <c r="P35">
         <v>782</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q35" s="5">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -2440,8 +2554,11 @@
       <c r="P36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q36" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>65</v>
       </c>
@@ -2490,8 +2607,11 @@
       <c r="P37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q37" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
@@ -2540,8 +2660,11 @@
       <c r="P38">
         <v>25</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q38" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>24</v>
       </c>
@@ -2590,8 +2713,11 @@
       <c r="P39">
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q39" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
@@ -2640,8 +2766,11 @@
       <c r="P40">
         <v>13</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q40" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -2690,8 +2819,11 @@
       <c r="P41">
         <v>35</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q41" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
@@ -2740,8 +2872,11 @@
       <c r="P42">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q42" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>60</v>
       </c>
@@ -2790,8 +2925,11 @@
       <c r="P43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q43" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>20</v>
       </c>
@@ -2840,8 +2978,11 @@
       <c r="P44">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q44" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -2890,8 +3031,11 @@
       <c r="P45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q45" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -2940,8 +3084,11 @@
       <c r="P46">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q46" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>12</v>
       </c>
@@ -2990,8 +3137,11 @@
       <c r="P47">
         <v>29</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q47" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -3040,8 +3190,11 @@
       <c r="P48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q48" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>21</v>
       </c>
@@ -3090,8 +3243,11 @@
       <c r="P49">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q49" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>16</v>
       </c>
@@ -3140,8 +3296,11 @@
       <c r="P50">
         <v>17</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q50" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>1</v>
       </c>
@@ -3190,8 +3349,11 @@
       <c r="P51">
         <v>191</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q51" s="5">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>66</v>
       </c>
@@ -3240,8 +3402,11 @@
       <c r="P52" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q52" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>18</v>
       </c>
@@ -3290,8 +3455,11 @@
       <c r="P53">
         <v>17</v>
       </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q53" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>67</v>
       </c>
@@ -3338,6 +3506,9 @@
         <v>0</v>
       </c>
       <c r="P54" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>